<commit_message>
Update reportes, botones documentacion estudiante y correccion de tildes
</commit_message>
<xml_diff>
--- a/public/Plantillas/HistoricoDocentes.xlsx
+++ b/public/Plantillas/HistoricoDocentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\TesisVersionBeta\Tesis_Final_Version\public\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tesis_version\tesis2\Tesis_Final_Version\public\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA32008-EE3D-4293-ACFE-5A9E4D48E630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608A7A1D-E916-44A6-A912-08D682B4EEE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA0A86E9-0812-4831-9BB8-61CEB0D52C2A}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{BA0A86E9-0812-4831-9BB8-61CEB0D52C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,31 +23,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ESPE ID</t>
   </si>
   <si>
-    <t xml:space="preserve">                              UNIVERSIDAD DE LAS FUERZAS ARMADAS - ESPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 CARRERA DE TECNOLOGÍAS DE LA INFORMACIÓN</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -108,10 +93,22 @@
     <t>NRC</t>
   </si>
   <si>
-    <t xml:space="preserve">REPORTE DE VINCULACIÓN </t>
-  </si>
-  <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNIVERSIDAD DE LAS FUERZAS ARMADAS - ESPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 </t>
+  </si>
+  <si>
+    <t>CARRERA DE TECNOLOGÍAS DE LA INFORMACIÓN</t>
+  </si>
+  <si>
+    <t>REPORTE DE ESTUDIANTES DE SERVICIO COMUNITARIO</t>
   </si>
 </sst>
 </file>
@@ -184,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -206,6 +203,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,20 +229,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1424940</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1023216</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>99681</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1428750" cy="476250"/>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>486529</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88606</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB0551AD-F7BC-4342-81DD-54BA55DA9A62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80DAB86-1015-44BC-80A1-26A769C84220}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -253,15 +256,21 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8077200" y="251460"/>
-          <a:ext cx="1428750" cy="476250"/>
+          <a:off x="14167716" y="290181"/>
+          <a:ext cx="1535001" cy="655675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -269,7 +278,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -572,38 +581,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D8BC6F-F653-4F8F-B96E-D91D7F594A13}">
   <dimension ref="A3:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="10" width="21.77734375" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="14" width="37.5546875" customWidth="1"/>
-    <col min="15" max="15" width="40.44140625" customWidth="1"/>
-    <col min="16" max="17" width="36.6640625" customWidth="1"/>
-    <col min="18" max="19" width="32.33203125" customWidth="1"/>
-    <col min="20" max="21" width="18.44140625" customWidth="1"/>
-    <col min="22" max="22" width="16.33203125" customWidth="1"/>
+    <col min="13" max="14" width="37.5703125" customWidth="1"/>
+    <col min="15" max="15" width="40.42578125" customWidth="1"/>
+    <col min="16" max="17" width="36.7109375" customWidth="1"/>
+    <col min="18" max="19" width="32.28515625" customWidth="1"/>
+    <col min="20" max="21" width="18.42578125" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="E3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -614,29 +625,31 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.35">
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+    <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -660,75 +673,75 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="T8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -755,9 +768,9 @@
   </sheetData>
   <autoFilter ref="A8:V8" xr:uid="{A0D8BC6F-F653-4F8F-B96E-D91D7F594A13}"/>
   <mergeCells count="3">
-    <mergeCell ref="E3:P3"/>
-    <mergeCell ref="D4:R4"/>
     <mergeCell ref="A7:V7"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>